<commit_message>
Add Pause, cheat and bonus
</commit_message>
<xml_diff>
--- a/level.xlsx
+++ b/level.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\UHK\PRO2\2016\MyFlappy\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="level" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="8">
   <si>
     <t>W</t>
   </si>
@@ -368,8 +364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +542,9 @@
       <c r="I10" t="s">
         <v>0</v>
       </c>
+      <c r="N10" t="s">
+        <v>5</v>
+      </c>
       <c r="P10" t="s">
         <v>0</v>
       </c>
@@ -571,6 +570,9 @@
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
       <c r="P12" t="s">
         <v>0</v>
       </c>

</xml_diff>